<commit_message>
1726/code changes for product dependency test plan
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="CreateOrder" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -34,7 +35,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 2</t>
+    <t xml:space="preserve">Web Data 12</t>
   </si>
   <si>
     <t xml:space="preserve">Semi-monthly</t>
@@ -94,10 +95,43 @@
     <t xml:space="preserve">2</t>
   </si>
   <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Billing Category Product 5</t>
   </si>
   <si>
     <t xml:space="preserve">Billing Category Product 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo Holder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olivia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isabella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sophia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jayden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semi-monthle</t>
   </si>
 </sst>
 </file>
@@ -223,18 +257,18 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.0962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.19259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.9555555555556"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,28 +310,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMI11"/>
+  <dimension ref="A1:AMI12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.17407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9296296296296"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.2148148148148"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.42592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.27037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.5814814814815"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6523,6 +6557,7 @@
       <c r="J7" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="K7" s="0"/>
       <c r="L7" s="0" t="s">
         <v>6</v>
       </c>
@@ -7549,6 +7584,9 @@
       <c r="H8" s="0"/>
       <c r="I8" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>19</v>
@@ -9607,7 +9645,7 @@
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
       <c r="E10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -9620,6 +9658,7 @@
       <c r="J10" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="K10" s="0"/>
       <c r="L10" s="0" t="s">
         <v>6</v>
       </c>
@@ -10641,15 +10680,25 @@
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="H11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I11" s="0"/>
-      <c r="L11" s="0"/>
+      <c r="I11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
       <c r="O11" s="0"/>
@@ -11662,6 +11711,1039 @@
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
     </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
+      <c r="T12" s="0"/>
+      <c r="U12" s="0"/>
+      <c r="V12" s="0"/>
+      <c r="W12" s="0"/>
+      <c r="X12" s="0"/>
+      <c r="Y12" s="0"/>
+      <c r="Z12" s="0"/>
+      <c r="AA12" s="0"/>
+      <c r="AB12" s="0"/>
+      <c r="AC12" s="0"/>
+      <c r="AD12" s="0"/>
+      <c r="AE12" s="0"/>
+      <c r="AF12" s="0"/>
+      <c r="AG12" s="0"/>
+      <c r="AH12" s="0"/>
+      <c r="AI12" s="0"/>
+      <c r="AJ12" s="0"/>
+      <c r="AK12" s="0"/>
+      <c r="AL12" s="0"/>
+      <c r="AM12" s="0"/>
+      <c r="AN12" s="0"/>
+      <c r="AO12" s="0"/>
+      <c r="AP12" s="0"/>
+      <c r="AQ12" s="0"/>
+      <c r="AR12" s="0"/>
+      <c r="AS12" s="0"/>
+      <c r="AT12" s="0"/>
+      <c r="AU12" s="0"/>
+      <c r="AV12" s="0"/>
+      <c r="AW12" s="0"/>
+      <c r="AX12" s="0"/>
+      <c r="AY12" s="0"/>
+      <c r="AZ12" s="0"/>
+      <c r="BA12" s="0"/>
+      <c r="BB12" s="0"/>
+      <c r="BC12" s="0"/>
+      <c r="BD12" s="0"/>
+      <c r="BE12" s="0"/>
+      <c r="BF12" s="0"/>
+      <c r="BG12" s="0"/>
+      <c r="BH12" s="0"/>
+      <c r="BI12" s="0"/>
+      <c r="BJ12" s="0"/>
+      <c r="BK12" s="0"/>
+      <c r="BL12" s="0"/>
+      <c r="BM12" s="0"/>
+      <c r="BN12" s="0"/>
+      <c r="BO12" s="0"/>
+      <c r="BP12" s="0"/>
+      <c r="BQ12" s="0"/>
+      <c r="BR12" s="0"/>
+      <c r="BS12" s="0"/>
+      <c r="BT12" s="0"/>
+      <c r="BU12" s="0"/>
+      <c r="BV12" s="0"/>
+      <c r="BW12" s="0"/>
+      <c r="BX12" s="0"/>
+      <c r="BY12" s="0"/>
+      <c r="BZ12" s="0"/>
+      <c r="CA12" s="0"/>
+      <c r="CB12" s="0"/>
+      <c r="CC12" s="0"/>
+      <c r="CD12" s="0"/>
+      <c r="CE12" s="0"/>
+      <c r="CF12" s="0"/>
+      <c r="CG12" s="0"/>
+      <c r="CH12" s="0"/>
+      <c r="CI12" s="0"/>
+      <c r="CJ12" s="0"/>
+      <c r="CK12" s="0"/>
+      <c r="CL12" s="0"/>
+      <c r="CM12" s="0"/>
+      <c r="CN12" s="0"/>
+      <c r="CO12" s="0"/>
+      <c r="CP12" s="0"/>
+      <c r="CQ12" s="0"/>
+      <c r="CR12" s="0"/>
+      <c r="CS12" s="0"/>
+      <c r="CT12" s="0"/>
+      <c r="CU12" s="0"/>
+      <c r="CV12" s="0"/>
+      <c r="CW12" s="0"/>
+      <c r="CX12" s="0"/>
+      <c r="CY12" s="0"/>
+      <c r="CZ12" s="0"/>
+      <c r="DA12" s="0"/>
+      <c r="DB12" s="0"/>
+      <c r="DC12" s="0"/>
+      <c r="DD12" s="0"/>
+      <c r="DE12" s="0"/>
+      <c r="DF12" s="0"/>
+      <c r="DG12" s="0"/>
+      <c r="DH12" s="0"/>
+      <c r="DI12" s="0"/>
+      <c r="DJ12" s="0"/>
+      <c r="DK12" s="0"/>
+      <c r="DL12" s="0"/>
+      <c r="DM12" s="0"/>
+      <c r="DN12" s="0"/>
+      <c r="DO12" s="0"/>
+      <c r="DP12" s="0"/>
+      <c r="DQ12" s="0"/>
+      <c r="DR12" s="0"/>
+      <c r="DS12" s="0"/>
+      <c r="DT12" s="0"/>
+      <c r="DU12" s="0"/>
+      <c r="DV12" s="0"/>
+      <c r="DW12" s="0"/>
+      <c r="DX12" s="0"/>
+      <c r="DY12" s="0"/>
+      <c r="DZ12" s="0"/>
+      <c r="EA12" s="0"/>
+      <c r="EB12" s="0"/>
+      <c r="EC12" s="0"/>
+      <c r="ED12" s="0"/>
+      <c r="EE12" s="0"/>
+      <c r="EF12" s="0"/>
+      <c r="EG12" s="0"/>
+      <c r="EH12" s="0"/>
+      <c r="EI12" s="0"/>
+      <c r="EJ12" s="0"/>
+      <c r="EK12" s="0"/>
+      <c r="EL12" s="0"/>
+      <c r="EM12" s="0"/>
+      <c r="EN12" s="0"/>
+      <c r="EO12" s="0"/>
+      <c r="EP12" s="0"/>
+      <c r="EQ12" s="0"/>
+      <c r="ER12" s="0"/>
+      <c r="ES12" s="0"/>
+      <c r="ET12" s="0"/>
+      <c r="EU12" s="0"/>
+      <c r="EV12" s="0"/>
+      <c r="EW12" s="0"/>
+      <c r="EX12" s="0"/>
+      <c r="EY12" s="0"/>
+      <c r="EZ12" s="0"/>
+      <c r="FA12" s="0"/>
+      <c r="FB12" s="0"/>
+      <c r="FC12" s="0"/>
+      <c r="FD12" s="0"/>
+      <c r="FE12" s="0"/>
+      <c r="FF12" s="0"/>
+      <c r="FG12" s="0"/>
+      <c r="FH12" s="0"/>
+      <c r="FI12" s="0"/>
+      <c r="FJ12" s="0"/>
+      <c r="FK12" s="0"/>
+      <c r="FL12" s="0"/>
+      <c r="FM12" s="0"/>
+      <c r="FN12" s="0"/>
+      <c r="FO12" s="0"/>
+      <c r="FP12" s="0"/>
+      <c r="FQ12" s="0"/>
+      <c r="FR12" s="0"/>
+      <c r="FS12" s="0"/>
+      <c r="FT12" s="0"/>
+      <c r="FU12" s="0"/>
+      <c r="FV12" s="0"/>
+      <c r="FW12" s="0"/>
+      <c r="FX12" s="0"/>
+      <c r="FY12" s="0"/>
+      <c r="FZ12" s="0"/>
+      <c r="GA12" s="0"/>
+      <c r="GB12" s="0"/>
+      <c r="GC12" s="0"/>
+      <c r="GD12" s="0"/>
+      <c r="GE12" s="0"/>
+      <c r="GF12" s="0"/>
+      <c r="GG12" s="0"/>
+      <c r="GH12" s="0"/>
+      <c r="GI12" s="0"/>
+      <c r="GJ12" s="0"/>
+      <c r="GK12" s="0"/>
+      <c r="GL12" s="0"/>
+      <c r="GM12" s="0"/>
+      <c r="GN12" s="0"/>
+      <c r="GO12" s="0"/>
+      <c r="GP12" s="0"/>
+      <c r="GQ12" s="0"/>
+      <c r="GR12" s="0"/>
+      <c r="GS12" s="0"/>
+      <c r="GT12" s="0"/>
+      <c r="GU12" s="0"/>
+      <c r="GV12" s="0"/>
+      <c r="GW12" s="0"/>
+      <c r="GX12" s="0"/>
+      <c r="GY12" s="0"/>
+      <c r="GZ12" s="0"/>
+      <c r="HA12" s="0"/>
+      <c r="HB12" s="0"/>
+      <c r="HC12" s="0"/>
+      <c r="HD12" s="0"/>
+      <c r="HE12" s="0"/>
+      <c r="HF12" s="0"/>
+      <c r="HG12" s="0"/>
+      <c r="HH12" s="0"/>
+      <c r="HI12" s="0"/>
+      <c r="HJ12" s="0"/>
+      <c r="HK12" s="0"/>
+      <c r="HL12" s="0"/>
+      <c r="HM12" s="0"/>
+      <c r="HN12" s="0"/>
+      <c r="HO12" s="0"/>
+      <c r="HP12" s="0"/>
+      <c r="HQ12" s="0"/>
+      <c r="HR12" s="0"/>
+      <c r="HS12" s="0"/>
+      <c r="HT12" s="0"/>
+      <c r="HU12" s="0"/>
+      <c r="HV12" s="0"/>
+      <c r="HW12" s="0"/>
+      <c r="HX12" s="0"/>
+      <c r="HY12" s="0"/>
+      <c r="HZ12" s="0"/>
+      <c r="IA12" s="0"/>
+      <c r="IB12" s="0"/>
+      <c r="IC12" s="0"/>
+      <c r="ID12" s="0"/>
+      <c r="IE12" s="0"/>
+      <c r="IF12" s="0"/>
+      <c r="IG12" s="0"/>
+      <c r="IH12" s="0"/>
+      <c r="II12" s="0"/>
+      <c r="IJ12" s="0"/>
+      <c r="IK12" s="0"/>
+      <c r="IL12" s="0"/>
+      <c r="IM12" s="0"/>
+      <c r="IN12" s="0"/>
+      <c r="IO12" s="0"/>
+      <c r="IP12" s="0"/>
+      <c r="IQ12" s="0"/>
+      <c r="IR12" s="0"/>
+      <c r="IS12" s="0"/>
+      <c r="IT12" s="0"/>
+      <c r="IU12" s="0"/>
+      <c r="IV12" s="0"/>
+      <c r="IW12" s="0"/>
+      <c r="IX12" s="0"/>
+      <c r="IY12" s="0"/>
+      <c r="IZ12" s="0"/>
+      <c r="JA12" s="0"/>
+      <c r="JB12" s="0"/>
+      <c r="JC12" s="0"/>
+      <c r="JD12" s="0"/>
+      <c r="JE12" s="0"/>
+      <c r="JF12" s="0"/>
+      <c r="JG12" s="0"/>
+      <c r="JH12" s="0"/>
+      <c r="JI12" s="0"/>
+      <c r="JJ12" s="0"/>
+      <c r="JK12" s="0"/>
+      <c r="JL12" s="0"/>
+      <c r="JM12" s="0"/>
+      <c r="JN12" s="0"/>
+      <c r="JO12" s="0"/>
+      <c r="JP12" s="0"/>
+      <c r="JQ12" s="0"/>
+      <c r="JR12" s="0"/>
+      <c r="JS12" s="0"/>
+      <c r="JT12" s="0"/>
+      <c r="JU12" s="0"/>
+      <c r="JV12" s="0"/>
+      <c r="JW12" s="0"/>
+      <c r="JX12" s="0"/>
+      <c r="JY12" s="0"/>
+      <c r="JZ12" s="0"/>
+      <c r="KA12" s="0"/>
+      <c r="KB12" s="0"/>
+      <c r="KC12" s="0"/>
+      <c r="KD12" s="0"/>
+      <c r="KE12" s="0"/>
+      <c r="KF12" s="0"/>
+      <c r="KG12" s="0"/>
+      <c r="KH12" s="0"/>
+      <c r="KI12" s="0"/>
+      <c r="KJ12" s="0"/>
+      <c r="KK12" s="0"/>
+      <c r="KL12" s="0"/>
+      <c r="KM12" s="0"/>
+      <c r="KN12" s="0"/>
+      <c r="KO12" s="0"/>
+      <c r="KP12" s="0"/>
+      <c r="KQ12" s="0"/>
+      <c r="KR12" s="0"/>
+      <c r="KS12" s="0"/>
+      <c r="KT12" s="0"/>
+      <c r="KU12" s="0"/>
+      <c r="KV12" s="0"/>
+      <c r="KW12" s="0"/>
+      <c r="KX12" s="0"/>
+      <c r="KY12" s="0"/>
+      <c r="KZ12" s="0"/>
+      <c r="LA12" s="0"/>
+      <c r="LB12" s="0"/>
+      <c r="LC12" s="0"/>
+      <c r="LD12" s="0"/>
+      <c r="LE12" s="0"/>
+      <c r="LF12" s="0"/>
+      <c r="LG12" s="0"/>
+      <c r="LH12" s="0"/>
+      <c r="LI12" s="0"/>
+      <c r="LJ12" s="0"/>
+      <c r="LK12" s="0"/>
+      <c r="LL12" s="0"/>
+      <c r="LM12" s="0"/>
+      <c r="LN12" s="0"/>
+      <c r="LO12" s="0"/>
+      <c r="LP12" s="0"/>
+      <c r="LQ12" s="0"/>
+      <c r="LR12" s="0"/>
+      <c r="LS12" s="0"/>
+      <c r="LT12" s="0"/>
+      <c r="LU12" s="0"/>
+      <c r="LV12" s="0"/>
+      <c r="LW12" s="0"/>
+      <c r="LX12" s="0"/>
+      <c r="LY12" s="0"/>
+      <c r="LZ12" s="0"/>
+      <c r="MA12" s="0"/>
+      <c r="MB12" s="0"/>
+      <c r="MC12" s="0"/>
+      <c r="MD12" s="0"/>
+      <c r="ME12" s="0"/>
+      <c r="MF12" s="0"/>
+      <c r="MG12" s="0"/>
+      <c r="MH12" s="0"/>
+      <c r="MI12" s="0"/>
+      <c r="MJ12" s="0"/>
+      <c r="MK12" s="0"/>
+      <c r="ML12" s="0"/>
+      <c r="MM12" s="0"/>
+      <c r="MN12" s="0"/>
+      <c r="MO12" s="0"/>
+      <c r="MP12" s="0"/>
+      <c r="MQ12" s="0"/>
+      <c r="MR12" s="0"/>
+      <c r="MS12" s="0"/>
+      <c r="MT12" s="0"/>
+      <c r="MU12" s="0"/>
+      <c r="MV12" s="0"/>
+      <c r="MW12" s="0"/>
+      <c r="MX12" s="0"/>
+      <c r="MY12" s="0"/>
+      <c r="MZ12" s="0"/>
+      <c r="NA12" s="0"/>
+      <c r="NB12" s="0"/>
+      <c r="NC12" s="0"/>
+      <c r="ND12" s="0"/>
+      <c r="NE12" s="0"/>
+      <c r="NF12" s="0"/>
+      <c r="NG12" s="0"/>
+      <c r="NH12" s="0"/>
+      <c r="NI12" s="0"/>
+      <c r="NJ12" s="0"/>
+      <c r="NK12" s="0"/>
+      <c r="NL12" s="0"/>
+      <c r="NM12" s="0"/>
+      <c r="NN12" s="0"/>
+      <c r="NO12" s="0"/>
+      <c r="NP12" s="0"/>
+      <c r="NQ12" s="0"/>
+      <c r="NR12" s="0"/>
+      <c r="NS12" s="0"/>
+      <c r="NT12" s="0"/>
+      <c r="NU12" s="0"/>
+      <c r="NV12" s="0"/>
+      <c r="NW12" s="0"/>
+      <c r="NX12" s="0"/>
+      <c r="NY12" s="0"/>
+      <c r="NZ12" s="0"/>
+      <c r="OA12" s="0"/>
+      <c r="OB12" s="0"/>
+      <c r="OC12" s="0"/>
+      <c r="OD12" s="0"/>
+      <c r="OE12" s="0"/>
+      <c r="OF12" s="0"/>
+      <c r="OG12" s="0"/>
+      <c r="OH12" s="0"/>
+      <c r="OI12" s="0"/>
+      <c r="OJ12" s="0"/>
+      <c r="OK12" s="0"/>
+      <c r="OL12" s="0"/>
+      <c r="OM12" s="0"/>
+      <c r="ON12" s="0"/>
+      <c r="OO12" s="0"/>
+      <c r="OP12" s="0"/>
+      <c r="OQ12" s="0"/>
+      <c r="OR12" s="0"/>
+      <c r="OS12" s="0"/>
+      <c r="OT12" s="0"/>
+      <c r="OU12" s="0"/>
+      <c r="OV12" s="0"/>
+      <c r="OW12" s="0"/>
+      <c r="OX12" s="0"/>
+      <c r="OY12" s="0"/>
+      <c r="OZ12" s="0"/>
+      <c r="PA12" s="0"/>
+      <c r="PB12" s="0"/>
+      <c r="PC12" s="0"/>
+      <c r="PD12" s="0"/>
+      <c r="PE12" s="0"/>
+      <c r="PF12" s="0"/>
+      <c r="PG12" s="0"/>
+      <c r="PH12" s="0"/>
+      <c r="PI12" s="0"/>
+      <c r="PJ12" s="0"/>
+      <c r="PK12" s="0"/>
+      <c r="PL12" s="0"/>
+      <c r="PM12" s="0"/>
+      <c r="PN12" s="0"/>
+      <c r="PO12" s="0"/>
+      <c r="PP12" s="0"/>
+      <c r="PQ12" s="0"/>
+      <c r="PR12" s="0"/>
+      <c r="PS12" s="0"/>
+      <c r="PT12" s="0"/>
+      <c r="PU12" s="0"/>
+      <c r="PV12" s="0"/>
+      <c r="PW12" s="0"/>
+      <c r="PX12" s="0"/>
+      <c r="PY12" s="0"/>
+      <c r="PZ12" s="0"/>
+      <c r="QA12" s="0"/>
+      <c r="QB12" s="0"/>
+      <c r="QC12" s="0"/>
+      <c r="QD12" s="0"/>
+      <c r="QE12" s="0"/>
+      <c r="QF12" s="0"/>
+      <c r="QG12" s="0"/>
+      <c r="QH12" s="0"/>
+      <c r="QI12" s="0"/>
+      <c r="QJ12" s="0"/>
+      <c r="QK12" s="0"/>
+      <c r="QL12" s="0"/>
+      <c r="QM12" s="0"/>
+      <c r="QN12" s="0"/>
+      <c r="QO12" s="0"/>
+      <c r="QP12" s="0"/>
+      <c r="QQ12" s="0"/>
+      <c r="QR12" s="0"/>
+      <c r="QS12" s="0"/>
+      <c r="QT12" s="0"/>
+      <c r="QU12" s="0"/>
+      <c r="QV12" s="0"/>
+      <c r="QW12" s="0"/>
+      <c r="QX12" s="0"/>
+      <c r="QY12" s="0"/>
+      <c r="QZ12" s="0"/>
+      <c r="RA12" s="0"/>
+      <c r="RB12" s="0"/>
+      <c r="RC12" s="0"/>
+      <c r="RD12" s="0"/>
+      <c r="RE12" s="0"/>
+      <c r="RF12" s="0"/>
+      <c r="RG12" s="0"/>
+      <c r="RH12" s="0"/>
+      <c r="RI12" s="0"/>
+      <c r="RJ12" s="0"/>
+      <c r="RK12" s="0"/>
+      <c r="RL12" s="0"/>
+      <c r="RM12" s="0"/>
+      <c r="RN12" s="0"/>
+      <c r="RO12" s="0"/>
+      <c r="RP12" s="0"/>
+      <c r="RQ12" s="0"/>
+      <c r="RR12" s="0"/>
+      <c r="RS12" s="0"/>
+      <c r="RT12" s="0"/>
+      <c r="RU12" s="0"/>
+      <c r="RV12" s="0"/>
+      <c r="RW12" s="0"/>
+      <c r="RX12" s="0"/>
+      <c r="RY12" s="0"/>
+      <c r="RZ12" s="0"/>
+      <c r="SA12" s="0"/>
+      <c r="SB12" s="0"/>
+      <c r="SC12" s="0"/>
+      <c r="SD12" s="0"/>
+      <c r="SE12" s="0"/>
+      <c r="SF12" s="0"/>
+      <c r="SG12" s="0"/>
+      <c r="SH12" s="0"/>
+      <c r="SI12" s="0"/>
+      <c r="SJ12" s="0"/>
+      <c r="SK12" s="0"/>
+      <c r="SL12" s="0"/>
+      <c r="SM12" s="0"/>
+      <c r="SN12" s="0"/>
+      <c r="SO12" s="0"/>
+      <c r="SP12" s="0"/>
+      <c r="SQ12" s="0"/>
+      <c r="SR12" s="0"/>
+      <c r="SS12" s="0"/>
+      <c r="ST12" s="0"/>
+      <c r="SU12" s="0"/>
+      <c r="SV12" s="0"/>
+      <c r="SW12" s="0"/>
+      <c r="SX12" s="0"/>
+      <c r="SY12" s="0"/>
+      <c r="SZ12" s="0"/>
+      <c r="TA12" s="0"/>
+      <c r="TB12" s="0"/>
+      <c r="TC12" s="0"/>
+      <c r="TD12" s="0"/>
+      <c r="TE12" s="0"/>
+      <c r="TF12" s="0"/>
+      <c r="TG12" s="0"/>
+      <c r="TH12" s="0"/>
+      <c r="TI12" s="0"/>
+      <c r="TJ12" s="0"/>
+      <c r="TK12" s="0"/>
+      <c r="TL12" s="0"/>
+      <c r="TM12" s="0"/>
+      <c r="TN12" s="0"/>
+      <c r="TO12" s="0"/>
+      <c r="TP12" s="0"/>
+      <c r="TQ12" s="0"/>
+      <c r="TR12" s="0"/>
+      <c r="TS12" s="0"/>
+      <c r="TT12" s="0"/>
+      <c r="TU12" s="0"/>
+      <c r="TV12" s="0"/>
+      <c r="TW12" s="0"/>
+      <c r="TX12" s="0"/>
+      <c r="TY12" s="0"/>
+      <c r="TZ12" s="0"/>
+      <c r="UA12" s="0"/>
+      <c r="UB12" s="0"/>
+      <c r="UC12" s="0"/>
+      <c r="UD12" s="0"/>
+      <c r="UE12" s="0"/>
+      <c r="UF12" s="0"/>
+      <c r="UG12" s="0"/>
+      <c r="UH12" s="0"/>
+      <c r="UI12" s="0"/>
+      <c r="UJ12" s="0"/>
+      <c r="UK12" s="0"/>
+      <c r="UL12" s="0"/>
+      <c r="UM12" s="0"/>
+      <c r="UN12" s="0"/>
+      <c r="UO12" s="0"/>
+      <c r="UP12" s="0"/>
+      <c r="UQ12" s="0"/>
+      <c r="UR12" s="0"/>
+      <c r="US12" s="0"/>
+      <c r="UT12" s="0"/>
+      <c r="UU12" s="0"/>
+      <c r="UV12" s="0"/>
+      <c r="UW12" s="0"/>
+      <c r="UX12" s="0"/>
+      <c r="UY12" s="0"/>
+      <c r="UZ12" s="0"/>
+      <c r="VA12" s="0"/>
+      <c r="VB12" s="0"/>
+      <c r="VC12" s="0"/>
+      <c r="VD12" s="0"/>
+      <c r="VE12" s="0"/>
+      <c r="VF12" s="0"/>
+      <c r="VG12" s="0"/>
+      <c r="VH12" s="0"/>
+      <c r="VI12" s="0"/>
+      <c r="VJ12" s="0"/>
+      <c r="VK12" s="0"/>
+      <c r="VL12" s="0"/>
+      <c r="VM12" s="0"/>
+      <c r="VN12" s="0"/>
+      <c r="VO12" s="0"/>
+      <c r="VP12" s="0"/>
+      <c r="VQ12" s="0"/>
+      <c r="VR12" s="0"/>
+      <c r="VS12" s="0"/>
+      <c r="VT12" s="0"/>
+      <c r="VU12" s="0"/>
+      <c r="VV12" s="0"/>
+      <c r="VW12" s="0"/>
+      <c r="VX12" s="0"/>
+      <c r="VY12" s="0"/>
+      <c r="VZ12" s="0"/>
+      <c r="WA12" s="0"/>
+      <c r="WB12" s="0"/>
+      <c r="WC12" s="0"/>
+      <c r="WD12" s="0"/>
+      <c r="WE12" s="0"/>
+      <c r="WF12" s="0"/>
+      <c r="WG12" s="0"/>
+      <c r="WH12" s="0"/>
+      <c r="WI12" s="0"/>
+      <c r="WJ12" s="0"/>
+      <c r="WK12" s="0"/>
+      <c r="WL12" s="0"/>
+      <c r="WM12" s="0"/>
+      <c r="WN12" s="0"/>
+      <c r="WO12" s="0"/>
+      <c r="WP12" s="0"/>
+      <c r="WQ12" s="0"/>
+      <c r="WR12" s="0"/>
+      <c r="WS12" s="0"/>
+      <c r="WT12" s="0"/>
+      <c r="WU12" s="0"/>
+      <c r="WV12" s="0"/>
+      <c r="WW12" s="0"/>
+      <c r="WX12" s="0"/>
+      <c r="WY12" s="0"/>
+      <c r="WZ12" s="0"/>
+      <c r="XA12" s="0"/>
+      <c r="XB12" s="0"/>
+      <c r="XC12" s="0"/>
+      <c r="XD12" s="0"/>
+      <c r="XE12" s="0"/>
+      <c r="XF12" s="0"/>
+      <c r="XG12" s="0"/>
+      <c r="XH12" s="0"/>
+      <c r="XI12" s="0"/>
+      <c r="XJ12" s="0"/>
+      <c r="XK12" s="0"/>
+      <c r="XL12" s="0"/>
+      <c r="XM12" s="0"/>
+      <c r="XN12" s="0"/>
+      <c r="XO12" s="0"/>
+      <c r="XP12" s="0"/>
+      <c r="XQ12" s="0"/>
+      <c r="XR12" s="0"/>
+      <c r="XS12" s="0"/>
+      <c r="XT12" s="0"/>
+      <c r="XU12" s="0"/>
+      <c r="XV12" s="0"/>
+      <c r="XW12" s="0"/>
+      <c r="XX12" s="0"/>
+      <c r="XY12" s="0"/>
+      <c r="XZ12" s="0"/>
+      <c r="YA12" s="0"/>
+      <c r="YB12" s="0"/>
+      <c r="YC12" s="0"/>
+      <c r="YD12" s="0"/>
+      <c r="YE12" s="0"/>
+      <c r="YF12" s="0"/>
+      <c r="YG12" s="0"/>
+      <c r="YH12" s="0"/>
+      <c r="YI12" s="0"/>
+      <c r="YJ12" s="0"/>
+      <c r="YK12" s="0"/>
+      <c r="YL12" s="0"/>
+      <c r="YM12" s="0"/>
+      <c r="YN12" s="0"/>
+      <c r="YO12" s="0"/>
+      <c r="YP12" s="0"/>
+      <c r="YQ12" s="0"/>
+      <c r="YR12" s="0"/>
+      <c r="YS12" s="0"/>
+      <c r="YT12" s="0"/>
+      <c r="YU12" s="0"/>
+      <c r="YV12" s="0"/>
+      <c r="YW12" s="0"/>
+      <c r="YX12" s="0"/>
+      <c r="YY12" s="0"/>
+      <c r="YZ12" s="0"/>
+      <c r="ZA12" s="0"/>
+      <c r="ZB12" s="0"/>
+      <c r="ZC12" s="0"/>
+      <c r="ZD12" s="0"/>
+      <c r="ZE12" s="0"/>
+      <c r="ZF12" s="0"/>
+      <c r="ZG12" s="0"/>
+      <c r="ZH12" s="0"/>
+      <c r="ZI12" s="0"/>
+      <c r="ZJ12" s="0"/>
+      <c r="ZK12" s="0"/>
+      <c r="ZL12" s="0"/>
+      <c r="ZM12" s="0"/>
+      <c r="ZN12" s="0"/>
+      <c r="ZO12" s="0"/>
+      <c r="ZP12" s="0"/>
+      <c r="ZQ12" s="0"/>
+      <c r="ZR12" s="0"/>
+      <c r="ZS12" s="0"/>
+      <c r="ZT12" s="0"/>
+      <c r="ZU12" s="0"/>
+      <c r="ZV12" s="0"/>
+      <c r="ZW12" s="0"/>
+      <c r="ZX12" s="0"/>
+      <c r="ZY12" s="0"/>
+      <c r="ZZ12" s="0"/>
+      <c r="AAA12" s="0"/>
+      <c r="AAB12" s="0"/>
+      <c r="AAC12" s="0"/>
+      <c r="AAD12" s="0"/>
+      <c r="AAE12" s="0"/>
+      <c r="AAF12" s="0"/>
+      <c r="AAG12" s="0"/>
+      <c r="AAH12" s="0"/>
+      <c r="AAI12" s="0"/>
+      <c r="AAJ12" s="0"/>
+      <c r="AAK12" s="0"/>
+      <c r="AAL12" s="0"/>
+      <c r="AAM12" s="0"/>
+      <c r="AAN12" s="0"/>
+      <c r="AAO12" s="0"/>
+      <c r="AAP12" s="0"/>
+      <c r="AAQ12" s="0"/>
+      <c r="AAR12" s="0"/>
+      <c r="AAS12" s="0"/>
+      <c r="AAT12" s="0"/>
+      <c r="AAU12" s="0"/>
+      <c r="AAV12" s="0"/>
+      <c r="AAW12" s="0"/>
+      <c r="AAX12" s="0"/>
+      <c r="AAY12" s="0"/>
+      <c r="AAZ12" s="0"/>
+      <c r="ABA12" s="0"/>
+      <c r="ABB12" s="0"/>
+      <c r="ABC12" s="0"/>
+      <c r="ABD12" s="0"/>
+      <c r="ABE12" s="0"/>
+      <c r="ABF12" s="0"/>
+      <c r="ABG12" s="0"/>
+      <c r="ABH12" s="0"/>
+      <c r="ABI12" s="0"/>
+      <c r="ABJ12" s="0"/>
+      <c r="ABK12" s="0"/>
+      <c r="ABL12" s="0"/>
+      <c r="ABM12" s="0"/>
+      <c r="ABN12" s="0"/>
+      <c r="ABO12" s="0"/>
+      <c r="ABP12" s="0"/>
+      <c r="ABQ12" s="0"/>
+      <c r="ABR12" s="0"/>
+      <c r="ABS12" s="0"/>
+      <c r="ABT12" s="0"/>
+      <c r="ABU12" s="0"/>
+      <c r="ABV12" s="0"/>
+      <c r="ABW12" s="0"/>
+      <c r="ABX12" s="0"/>
+      <c r="ABY12" s="0"/>
+      <c r="ABZ12" s="0"/>
+      <c r="ACA12" s="0"/>
+      <c r="ACB12" s="0"/>
+      <c r="ACC12" s="0"/>
+      <c r="ACD12" s="0"/>
+      <c r="ACE12" s="0"/>
+      <c r="ACF12" s="0"/>
+      <c r="ACG12" s="0"/>
+      <c r="ACH12" s="0"/>
+      <c r="ACI12" s="0"/>
+      <c r="ACJ12" s="0"/>
+      <c r="ACK12" s="0"/>
+      <c r="ACL12" s="0"/>
+      <c r="ACM12" s="0"/>
+      <c r="ACN12" s="0"/>
+      <c r="ACO12" s="0"/>
+      <c r="ACP12" s="0"/>
+      <c r="ACQ12" s="0"/>
+      <c r="ACR12" s="0"/>
+      <c r="ACS12" s="0"/>
+      <c r="ACT12" s="0"/>
+      <c r="ACU12" s="0"/>
+      <c r="ACV12" s="0"/>
+      <c r="ACW12" s="0"/>
+      <c r="ACX12" s="0"/>
+      <c r="ACY12" s="0"/>
+      <c r="ACZ12" s="0"/>
+      <c r="ADA12" s="0"/>
+      <c r="ADB12" s="0"/>
+      <c r="ADC12" s="0"/>
+      <c r="ADD12" s="0"/>
+      <c r="ADE12" s="0"/>
+      <c r="ADF12" s="0"/>
+      <c r="ADG12" s="0"/>
+      <c r="ADH12" s="0"/>
+      <c r="ADI12" s="0"/>
+      <c r="ADJ12" s="0"/>
+      <c r="ADK12" s="0"/>
+      <c r="ADL12" s="0"/>
+      <c r="ADM12" s="0"/>
+      <c r="ADN12" s="0"/>
+      <c r="ADO12" s="0"/>
+      <c r="ADP12" s="0"/>
+      <c r="ADQ12" s="0"/>
+      <c r="ADR12" s="0"/>
+      <c r="ADS12" s="0"/>
+      <c r="ADT12" s="0"/>
+      <c r="ADU12" s="0"/>
+      <c r="ADV12" s="0"/>
+      <c r="ADW12" s="0"/>
+      <c r="ADX12" s="0"/>
+      <c r="ADY12" s="0"/>
+      <c r="ADZ12" s="0"/>
+      <c r="AEA12" s="0"/>
+      <c r="AEB12" s="0"/>
+      <c r="AEC12" s="0"/>
+      <c r="AED12" s="0"/>
+      <c r="AEE12" s="0"/>
+      <c r="AEF12" s="0"/>
+      <c r="AEG12" s="0"/>
+      <c r="AEH12" s="0"/>
+      <c r="AEI12" s="0"/>
+      <c r="AEJ12" s="0"/>
+      <c r="AEK12" s="0"/>
+      <c r="AEL12" s="0"/>
+      <c r="AEM12" s="0"/>
+      <c r="AEN12" s="0"/>
+      <c r="AEO12" s="0"/>
+      <c r="AEP12" s="0"/>
+      <c r="AEQ12" s="0"/>
+      <c r="AER12" s="0"/>
+      <c r="AES12" s="0"/>
+      <c r="AET12" s="0"/>
+      <c r="AEU12" s="0"/>
+      <c r="AEV12" s="0"/>
+      <c r="AEW12" s="0"/>
+      <c r="AEX12" s="0"/>
+      <c r="AEY12" s="0"/>
+      <c r="AEZ12" s="0"/>
+      <c r="AFA12" s="0"/>
+      <c r="AFB12" s="0"/>
+      <c r="AFC12" s="0"/>
+      <c r="AFD12" s="0"/>
+      <c r="AFE12" s="0"/>
+      <c r="AFF12" s="0"/>
+      <c r="AFG12" s="0"/>
+      <c r="AFH12" s="0"/>
+      <c r="AFI12" s="0"/>
+      <c r="AFJ12" s="0"/>
+      <c r="AFK12" s="0"/>
+      <c r="AFL12" s="0"/>
+      <c r="AFM12" s="0"/>
+      <c r="AFN12" s="0"/>
+      <c r="AFO12" s="0"/>
+      <c r="AFP12" s="0"/>
+      <c r="AFQ12" s="0"/>
+      <c r="AFR12" s="0"/>
+      <c r="AFS12" s="0"/>
+      <c r="AFT12" s="0"/>
+      <c r="AFU12" s="0"/>
+      <c r="AFV12" s="0"/>
+      <c r="AFW12" s="0"/>
+      <c r="AFX12" s="0"/>
+      <c r="AFY12" s="0"/>
+      <c r="AFZ12" s="0"/>
+      <c r="AGA12" s="0"/>
+      <c r="AGB12" s="0"/>
+      <c r="AGC12" s="0"/>
+      <c r="AGD12" s="0"/>
+      <c r="AGE12" s="0"/>
+      <c r="AGF12" s="0"/>
+      <c r="AGG12" s="0"/>
+      <c r="AGH12" s="0"/>
+      <c r="AGI12" s="0"/>
+      <c r="AGJ12" s="0"/>
+      <c r="AGK12" s="0"/>
+      <c r="AGL12" s="0"/>
+      <c r="AGM12" s="0"/>
+      <c r="AGN12" s="0"/>
+      <c r="AGO12" s="0"/>
+      <c r="AGP12" s="0"/>
+      <c r="AGQ12" s="0"/>
+      <c r="AGR12" s="0"/>
+      <c r="AGS12" s="0"/>
+      <c r="AGT12" s="0"/>
+      <c r="AGU12" s="0"/>
+      <c r="AGV12" s="0"/>
+      <c r="AGW12" s="0"/>
+      <c r="AGX12" s="0"/>
+      <c r="AGY12" s="0"/>
+      <c r="AGZ12" s="0"/>
+      <c r="AHA12" s="0"/>
+      <c r="AHB12" s="0"/>
+      <c r="AHC12" s="0"/>
+      <c r="AHD12" s="0"/>
+      <c r="AHE12" s="0"/>
+      <c r="AHF12" s="0"/>
+      <c r="AHG12" s="0"/>
+      <c r="AHH12" s="0"/>
+      <c r="AHI12" s="0"/>
+      <c r="AHJ12" s="0"/>
+      <c r="AHK12" s="0"/>
+      <c r="AHL12" s="0"/>
+      <c r="AHM12" s="0"/>
+      <c r="AHN12" s="0"/>
+      <c r="AHO12" s="0"/>
+      <c r="AHP12" s="0"/>
+      <c r="AHQ12" s="0"/>
+      <c r="AHR12" s="0"/>
+      <c r="AHS12" s="0"/>
+      <c r="AHT12" s="0"/>
+      <c r="AHU12" s="0"/>
+      <c r="AHV12" s="0"/>
+      <c r="AHW12" s="0"/>
+      <c r="AHX12" s="0"/>
+      <c r="AHY12" s="0"/>
+      <c r="AHZ12" s="0"/>
+      <c r="AIA12" s="0"/>
+      <c r="AIB12" s="0"/>
+      <c r="AIC12" s="0"/>
+      <c r="AID12" s="0"/>
+      <c r="AIE12" s="0"/>
+      <c r="AIF12" s="0"/>
+      <c r="AIG12" s="0"/>
+      <c r="AIH12" s="0"/>
+      <c r="AII12" s="0"/>
+      <c r="AIJ12" s="0"/>
+      <c r="AIK12" s="0"/>
+      <c r="AIL12" s="0"/>
+      <c r="AIM12" s="0"/>
+      <c r="AIN12" s="0"/>
+      <c r="AIO12" s="0"/>
+      <c r="AIP12" s="0"/>
+      <c r="AIQ12" s="0"/>
+      <c r="AIR12" s="0"/>
+      <c r="AIS12" s="0"/>
+      <c r="AIT12" s="0"/>
+      <c r="AIU12" s="0"/>
+      <c r="AIV12" s="0"/>
+      <c r="AIW12" s="0"/>
+      <c r="AIX12" s="0"/>
+      <c r="AIY12" s="0"/>
+      <c r="AIZ12" s="0"/>
+      <c r="AJA12" s="0"/>
+      <c r="AJB12" s="0"/>
+      <c r="AJC12" s="0"/>
+      <c r="AJD12" s="0"/>
+      <c r="AJE12" s="0"/>
+      <c r="AJF12" s="0"/>
+      <c r="AJG12" s="0"/>
+      <c r="AJH12" s="0"/>
+      <c r="AJI12" s="0"/>
+      <c r="AJJ12" s="0"/>
+      <c r="AJK12" s="0"/>
+      <c r="AJL12" s="0"/>
+      <c r="AJM12" s="0"/>
+      <c r="AJN12" s="0"/>
+      <c r="AJO12" s="0"/>
+      <c r="AJP12" s="0"/>
+      <c r="AJQ12" s="0"/>
+      <c r="AJR12" s="0"/>
+      <c r="AJS12" s="0"/>
+      <c r="AJT12" s="0"/>
+      <c r="AJU12" s="0"/>
+      <c r="AJV12" s="0"/>
+      <c r="AJW12" s="0"/>
+      <c r="AJX12" s="0"/>
+      <c r="AJY12" s="0"/>
+      <c r="AJZ12" s="0"/>
+      <c r="AKA12" s="0"/>
+      <c r="AKB12" s="0"/>
+      <c r="AKC12" s="0"/>
+      <c r="AKD12" s="0"/>
+      <c r="AKE12" s="0"/>
+      <c r="AKF12" s="0"/>
+      <c r="AKG12" s="0"/>
+      <c r="AKH12" s="0"/>
+      <c r="AKI12" s="0"/>
+      <c r="AKJ12" s="0"/>
+      <c r="AKK12" s="0"/>
+      <c r="AKL12" s="0"/>
+      <c r="AKM12" s="0"/>
+      <c r="AKN12" s="0"/>
+      <c r="AKO12" s="0"/>
+      <c r="AKP12" s="0"/>
+      <c r="AKQ12" s="0"/>
+      <c r="AKR12" s="0"/>
+      <c r="AKS12" s="0"/>
+      <c r="AKT12" s="0"/>
+      <c r="AKU12" s="0"/>
+      <c r="AKV12" s="0"/>
+      <c r="AKW12" s="0"/>
+      <c r="AKX12" s="0"/>
+      <c r="AKY12" s="0"/>
+      <c r="AKZ12" s="0"/>
+      <c r="ALA12" s="0"/>
+      <c r="ALB12" s="0"/>
+      <c r="ALC12" s="0"/>
+      <c r="ALD12" s="0"/>
+      <c r="ALE12" s="0"/>
+      <c r="ALF12" s="0"/>
+      <c r="ALG12" s="0"/>
+      <c r="ALH12" s="0"/>
+      <c r="ALI12" s="0"/>
+      <c r="ALJ12" s="0"/>
+      <c r="ALK12" s="0"/>
+      <c r="ALL12" s="0"/>
+      <c r="ALM12" s="0"/>
+      <c r="ALN12" s="0"/>
+      <c r="ALO12" s="0"/>
+      <c r="ALP12" s="0"/>
+      <c r="ALQ12" s="0"/>
+      <c r="ALR12" s="0"/>
+      <c r="ALS12" s="0"/>
+      <c r="ALT12" s="0"/>
+      <c r="ALU12" s="0"/>
+      <c r="ALV12" s="0"/>
+      <c r="ALW12" s="0"/>
+      <c r="ALX12" s="0"/>
+      <c r="ALY12" s="0"/>
+      <c r="ALZ12" s="0"/>
+      <c r="AMA12" s="0"/>
+      <c r="AMB12" s="0"/>
+      <c r="AMC12" s="0"/>
+      <c r="AMD12" s="0"/>
+      <c r="AME12" s="0"/>
+      <c r="AMF12" s="0"/>
+      <c r="AMG12" s="0"/>
+      <c r="AMH12" s="0"/>
+      <c r="AMI12" s="0"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
@@ -11681,27 +12763,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="F1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.0740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F1" s="4"/>
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -11717,39 +12849,102 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="E1:M2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.6666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.5407407407407"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.07407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.3259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.1888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3814814814815"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E1" s="3"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="n">
+        <v>2</v>
+      </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added functions to: * click Customer name * create order test plan * more utility functions and test plans
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -16,6 +16,8 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -131,7 +133,10 @@
     <t xml:space="preserve">pre paid</t>
   </si>
   <si>
-    <t xml:space="preserve">Semi-monthle</t>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post paid</t>
   </si>
 </sst>
 </file>
@@ -262,13 +267,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.19259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.38888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="12.4444444444444"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,20 +323,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.42592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.27037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.5814814814815"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.56666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12766,18 +12771,18 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12849,29 +12854,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.07407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.3259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.1888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3814814814815"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.9518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.76296296296296"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12899,8 +12904,8 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="n">
-        <v>2</v>
+      <c r="I1" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -12912,19 +12917,25 @@
       <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
       <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>33</v>
@@ -12935,10 +12946,135 @@
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="0"/>
       <c r="H4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create order for dependent product
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -39,7 +39,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 15</t>
+    <t xml:space="preserve">Web Data 18</t>
   </si>
   <si>
     <t xml:space="preserve">Semi-monthly</t>
@@ -311,7 +311,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -540,7 +540,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Changesin code according to code review comments
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,8 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -39,7 +41,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 18</t>
+    <t xml:space="preserve">Web Data 20</t>
   </si>
   <si>
     <t xml:space="preserve">Semi-monthly</t>
@@ -48,7 +50,7 @@
     <t xml:space="preserve">Semi-Monthly</t>
   </si>
   <si>
-    <t xml:space="preserve">Services 2</t>
+    <t xml:space="preserve">Services</t>
   </si>
   <si>
     <t xml:space="preserve">Billing Product 1</t>
@@ -260,13 +262,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.58518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.78148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.4259259259259"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -310,23 +312,23 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.25185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -368,6 +370,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="0"/>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
@@ -415,6 +418,14 @@
       <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0"/>
+      <c r="G8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0"/>
+      <c r="G9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
@@ -454,18 +465,18 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="12.6407407407407"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,26 +550,26 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.6740740740741"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.5"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.0481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.9111111111111"/>
+    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="12.6407407407407"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
changes into code before addition of  validation
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,6 +22,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -262,13 +263,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.7185185185185"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -312,23 +313,23 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.25185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.34814814814815"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,6 +360,7 @@
       <c r="M1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="0"/>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
@@ -464,19 +466,19 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="12.837037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,25 +553,25 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.0481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.9111111111111"/>
-    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.4851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.6333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.5"/>
+    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="12.837037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
insert validation into code
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,6 +23,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -130,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">pre paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$60.00</t>
   </si>
   <si>
     <t xml:space="preserve">post paid</t>
@@ -263,13 +267,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.88148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.97777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="14.0148148148148"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,17 +323,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.8888888888889"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.6703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.44814814814815"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,19 +470,19 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.1296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,26 +556,26 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.4851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.6333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.5"/>
-    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.2222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.0851851851852"/>
+    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="13.1296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -599,7 +603,9 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -612,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Added Validations In All Test Scenario
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t xml:space="preserve">pre paid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$60.00</t>
   </si>
   <si>
     <t xml:space="preserve">post paid</t>
@@ -557,7 +554,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -603,9 +600,7 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -618,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Comment the Company login call from the Scenario4
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,15 +15,6 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -35,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -50,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Semi-Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">Services</t>
@@ -258,19 +252,19 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.97777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="14.0148148148148"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="14.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,8 +283,8 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="n">
-        <v>1</v>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -299,7 +293,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -314,23 +308,23 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.6703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.40740740740741"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="10" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,41 +338,41 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="0"/>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="0"/>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>3</v>
@@ -386,40 +380,40 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,18 +426,18 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -452,7 +446,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -467,19 +461,19 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.1296296296296"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,43 +487,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +532,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -553,26 +547,26 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.2222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.0851851851852"/>
-    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="13.1296296296296"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="13" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="13.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -586,19 +580,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -607,61 +601,61 @@
     </row>
     <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +664,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added Filter for Customer in the Product Dependency Feature
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 20</t>
+    <t xml:space="preserve">Web Data 49</t>
   </si>
   <si>
     <t xml:space="preserve">Semi-monthly</t>
@@ -100,25 +100,43 @@
     <t xml:space="preserve">Billing Category Product 6</t>
   </si>
   <si>
-    <t xml:space="preserve">Direct Customer</t>
+    <t xml:space="preserve">LEO HOLDER</t>
   </si>
   <si>
     <t xml:space="preserve">Leo Holder</t>
   </si>
   <si>
+    <t xml:space="preserve">WILLIAM</t>
+  </si>
+  <si>
     <t xml:space="preserve">William</t>
   </si>
   <si>
+    <t xml:space="preserve">OLIVIA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Olivia</t>
   </si>
   <si>
+    <t xml:space="preserve">ISABELLA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Isabella</t>
   </si>
   <si>
+    <t xml:space="preserve">SOPHIA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sophia</t>
   </si>
   <si>
+    <t xml:space="preserve">JACOB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jacob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JAYDEN</t>
   </si>
   <si>
     <t xml:space="preserve">Jayden</t>
@@ -252,8 +270,8 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -262,8 +280,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="14.01"/>
   </cols>
   <sheetData>
@@ -320,8 +338,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="10" style="1" width="13.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.41"/>
@@ -462,7 +480,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -470,8 +488,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="20.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.13"/>
   </cols>
@@ -497,33 +514,51 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -547,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -559,8 +594,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.7"/>
@@ -586,7 +621,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>17</v>
@@ -601,13 +636,13 @@
     </row>
     <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
@@ -618,7 +653,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -633,7 +668,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="1" t="s">
@@ -642,7 +677,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="1" t="s">
@@ -651,7 +686,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="1" t="s">

</xml_diff>

<commit_message>
Added Validation for the order Period in the Product Dependency Feature
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 49</t>
+    <t xml:space="preserve">Web Data 1</t>
   </si>
   <si>
     <t xml:space="preserve">Semi-monthly</t>
@@ -270,7 +270,7 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -582,8 +582,8 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Chnage the amount of the Invoice Price according to the Test Plan
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,138 +14,134 @@
     <sheet name="CreateOrder" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$15:$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$13:$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$13:$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WebData@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Data 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semi-monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semi-Monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Product 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States Dollar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Product 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Product 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dependent Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEO HOLDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leo Holder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WILLIAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OLIVIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olivia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISABELLA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isabella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOPHIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sophia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JACOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jacob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAYDEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jayden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pre paid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post paid</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>WebData@123</t>
+  </si>
+  <si>
+    <t>Web Data 1</t>
+  </si>
+  <si>
+    <t>Semi-monthly</t>
+  </si>
+  <si>
+    <t>Semi-Monthly</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Dependent Product 1</t>
+  </si>
+  <si>
+    <t>United States Dollar</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Dependent Product 2</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>One time</t>
+  </si>
+  <si>
+    <t>Dependent Product 3</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Dependent Category</t>
+  </si>
+  <si>
+    <t>Dependent Category Product 1</t>
+  </si>
+  <si>
+    <t>Dependent Category Product 2</t>
+  </si>
+  <si>
+    <t>Dependent Category Product 3</t>
+  </si>
+  <si>
+    <t>Dependent Category Product 4</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Dependent Category Product 5</t>
+  </si>
+  <si>
+    <t>Dependent Category Product 6</t>
+  </si>
+  <si>
+    <t>LEO HOLDER</t>
+  </si>
+  <si>
+    <t>Leo Holder</t>
+  </si>
+  <si>
+    <t>WILLIAM</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>OLIVIA</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>ISABELLA</t>
+  </si>
+  <si>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>SOPHIA</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>JACOB</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>JAYDEN</t>
+  </si>
+  <si>
+    <t>Jayden</t>
+  </si>
+  <si>
+    <t>pre paid</t>
+  </si>
+  <si>
+    <t>post paid</t>
   </si>
 </sst>
 </file>
@@ -153,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
@@ -270,19 +266,19 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="14.01"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.8074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.98888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="14.0148148148148"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,7 +307,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -324,25 +320,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="10" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.41"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.6703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.45925925925926"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7888888888889"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.41481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,26 +431,18 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="0"/>
-      <c r="G8" s="0"/>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="0"/>
-      <c r="G9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -464,7 +452,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -479,18 +467,18 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="20.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="20.6814814814815"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.1296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,7 +555,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -582,26 +570,26 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="13" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="13.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.3148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.337037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.2074074074074"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.4111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.0851851851852"/>
+    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="13.1296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -699,7 +687,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Reduce the Code for the Product Dependency Test Plan
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -9,20 +9,22 @@
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="AddProductCategory1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AddProductCategory" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="AddCustomer" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="CreateOrder" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$13:$13</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory1!$13:$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory!$13:$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory!$13:$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">AddProductCategory!$13:$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">AddProductCategory!$13:$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>admin</t>
   </si>
@@ -30,7 +32,7 @@
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Web Data 1</t>
+    <t>Web Data 11</t>
   </si>
   <si>
     <t>Semi-monthly</t>
@@ -96,46 +98,40 @@
     <t>Dependent Category Product 6</t>
   </si>
   <si>
-    <t>LEO HOLDER</t>
-  </si>
-  <si>
-    <t>Leo Holder</t>
-  </si>
-  <si>
-    <t>WILLIAM</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>OLIVIA</t>
-  </si>
-  <si>
-    <t>Olivia</t>
-  </si>
-  <si>
-    <t>ISABELLA</t>
-  </si>
-  <si>
-    <t>Isabella</t>
-  </si>
-  <si>
-    <t>SOPHIA</t>
-  </si>
-  <si>
-    <t>Sophia</t>
-  </si>
-  <si>
-    <t>JACOB</t>
-  </si>
-  <si>
-    <t>Jacob</t>
-  </si>
-  <si>
-    <t>JAYDEN</t>
-  </si>
-  <si>
-    <t>Jayden</t>
+    <t>LEO DEPENDENT</t>
+  </si>
+  <si>
+    <t>Leo Dependent</t>
+  </si>
+  <si>
+    <t>WILLIAM DEPENDENT</t>
+  </si>
+  <si>
+    <t>William Dependent</t>
+  </si>
+  <si>
+    <t>OLIVIA DEPENDENT</t>
+  </si>
+  <si>
+    <t>Olivia Dependent</t>
+  </si>
+  <si>
+    <t>ISABELLA DEPENDENT</t>
+  </si>
+  <si>
+    <t>Isabella Dependent</t>
+  </si>
+  <si>
+    <t>SOPHIA DEPENDENT</t>
+  </si>
+  <si>
+    <t>Sophia Dependent</t>
+  </si>
+  <si>
+    <t>JACOB DEPENDENT</t>
+  </si>
+  <si>
+    <t>Jacob Dependent</t>
   </si>
   <si>
     <t>pre paid</t>
@@ -323,7 +319,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -465,10 +461,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,7 +513,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
@@ -539,14 +535,6 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -570,8 +558,8 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -579,7 +567,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6814814814815"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7666666666667"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.3148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6814814814815"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.337037037037"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8444444444444"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.2074074074074"/>
@@ -609,7 +597,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>17</v>
@@ -630,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
@@ -654,7 +642,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Parameterized the value of ItemType  for the Product Dependency Test Plan
</commit_message>
<xml_diff>
--- a/ProductDependency_TestData.xlsx
+++ b/ProductDependency_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OrderPeriod" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,129 +15,131 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory!$13:$13</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">AddProductCategory!$13:$13</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">AddProductCategory!$13:$13</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">AddProductCategory!$13:$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>WebData@123</t>
-  </si>
-  <si>
-    <t>Web Data 11</t>
-  </si>
-  <si>
-    <t>Semi-monthly</t>
-  </si>
-  <si>
-    <t>Semi-Monthly</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>Dependent Product 1</t>
-  </si>
-  <si>
-    <t>United States Dollar</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>Dependent Product 2</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>One time</t>
-  </si>
-  <si>
-    <t>Dependent Product 3</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Dependent Category</t>
-  </si>
-  <si>
-    <t>Dependent Category Product 1</t>
-  </si>
-  <si>
-    <t>Dependent Category Product 2</t>
-  </si>
-  <si>
-    <t>Dependent Category Product 3</t>
-  </si>
-  <si>
-    <t>Dependent Category Product 4</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Dependent Category Product 5</t>
-  </si>
-  <si>
-    <t>Dependent Category Product 6</t>
-  </si>
-  <si>
-    <t>LEO DEPENDENT</t>
-  </si>
-  <si>
-    <t>Leo Dependent</t>
-  </si>
-  <si>
-    <t>WILLIAM DEPENDENT</t>
-  </si>
-  <si>
-    <t>William Dependent</t>
-  </si>
-  <si>
-    <t>OLIVIA DEPENDENT</t>
-  </si>
-  <si>
-    <t>Olivia Dependent</t>
-  </si>
-  <si>
-    <t>ISABELLA DEPENDENT</t>
-  </si>
-  <si>
-    <t>Isabella Dependent</t>
-  </si>
-  <si>
-    <t>SOPHIA DEPENDENT</t>
-  </si>
-  <si>
-    <t>Sophia Dependent</t>
-  </si>
-  <si>
-    <t>JACOB DEPENDENT</t>
-  </si>
-  <si>
-    <t>Jacob Dependent</t>
-  </si>
-  <si>
-    <t>pre paid</t>
-  </si>
-  <si>
-    <t>post paid</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebData@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Data 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semi-monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semi-Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Product 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Product 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Product 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Category Product 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Category Product 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Category Product 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Category Product 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Category Product 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Category Product 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEO DEPENDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WILLIAM DEPENDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLIVIA DEPENDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olivia Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISABELLA DEPENDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isabella Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOPHIA DEPENDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sophia Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JACOB DEPENDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacob Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post paid</t>
   </si>
 </sst>
 </file>
@@ -145,7 +147,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
@@ -262,22 +264,22 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.8074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7888888888889"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.98888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="14.0148148148148"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="14.01"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -303,7 +305,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -318,23 +320,23 @@
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.6703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.45925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7888888888889"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.41481481481481"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="10" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,7 +450,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -463,18 +465,18 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="20.6814814814815"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.1296296296296"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,7 +545,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -558,26 +560,26 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.337037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.2074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.4111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.0851851851852"/>
-    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="13.1296296296296"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="13" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="13.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -605,7 +607,9 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -675,7 +679,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>